<commit_message>
Mayorista v3 corrección decimales en kg
</commit_message>
<xml_diff>
--- a/BD extracciones.xlsx
+++ b/BD extracciones.xlsx
@@ -438,11 +438,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L677"/>
+  <dimension ref="A1:L735"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F679" sqref="F679"/>
+      <pane ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A710" sqref="A710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -29762,6 +29762,2797 @@
       </c>
       <c r="K677" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="F678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="G678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="H678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="I678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="J678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="K678" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Barritas de submarino Aguila Caja (24 x 14 gr)</t>
+        </is>
+      </c>
+      <c r="C679" t="n">
+        <v>1</v>
+      </c>
+      <c r="D679" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="E679" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="F679" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G679" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H679" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I679" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="J679" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="K679" t="n">
+        <v>1</v>
+      </c>
+      <c r="L679" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Queso Crema Milka ut Balde x 3.6 Kg</t>
+        </is>
+      </c>
+      <c r="C680" t="n">
+        <v>2</v>
+      </c>
+      <c r="D680" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="E680" t="n">
+        <v>81397.06</v>
+      </c>
+      <c r="F680" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G680" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H680" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I680" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="J680" t="n">
+        <v>81397.06</v>
+      </c>
+      <c r="K680" t="n">
+        <v>2</v>
+      </c>
+      <c r="L680" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Rebozador Preferido Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C681" t="n">
+        <v>1</v>
+      </c>
+      <c r="D681" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E681" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="F681" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G681" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H681" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I681" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J681" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="K681" t="n">
+        <v>1</v>
+      </c>
+      <c r="L681" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Harina 000</t>
+        </is>
+      </c>
+      <c r="C682" t="n">
+        <v>100</v>
+      </c>
+      <c r="D682" t="n">
+        <v>250</v>
+      </c>
+      <c r="E682" t="n">
+        <v>25000</v>
+      </c>
+      <c r="F682" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G682" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H682" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I682" t="n">
+        <v>250</v>
+      </c>
+      <c r="J682" t="n">
+        <v>25000</v>
+      </c>
+      <c r="K682" t="n">
+        <v>100</v>
+      </c>
+      <c r="L682" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Azucar</t>
+        </is>
+      </c>
+      <c r="C683" t="n">
+        <v>50</v>
+      </c>
+      <c r="D683" t="n">
+        <v>120</v>
+      </c>
+      <c r="E683" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H683" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I683" t="n">
+        <v>120</v>
+      </c>
+      <c r="J683" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K683" t="n">
+        <v>50</v>
+      </c>
+      <c r="L683" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Levadura</t>
+        </is>
+      </c>
+      <c r="C684" t="n">
+        <v>2</v>
+      </c>
+      <c r="D684" t="n">
+        <v>350</v>
+      </c>
+      <c r="E684" t="n">
+        <v>700</v>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I684" t="n">
+        <v>350</v>
+      </c>
+      <c r="J684" t="n">
+        <v>700</v>
+      </c>
+      <c r="K684" t="n">
+        <v>2</v>
+      </c>
+      <c r="L684" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Sal</t>
+        </is>
+      </c>
+      <c r="C685" t="n">
+        <v>1</v>
+      </c>
+      <c r="D685" t="n">
+        <v>150</v>
+      </c>
+      <c r="E685" t="n">
+        <v>150</v>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H685" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I685" t="n">
+        <v>150</v>
+      </c>
+      <c r="J685" t="n">
+        <v>150</v>
+      </c>
+      <c r="K685" t="n">
+        <v>1</v>
+      </c>
+      <c r="L685" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Manteca</t>
+        </is>
+      </c>
+      <c r="C686" t="n">
+        <v>25</v>
+      </c>
+      <c r="D686" t="n">
+        <v>300</v>
+      </c>
+      <c r="E686" t="n">
+        <v>7500</v>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H686" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I686" t="n">
+        <v>300</v>
+      </c>
+      <c r="J686" t="n">
+        <v>7500</v>
+      </c>
+      <c r="K686" t="n">
+        <v>25</v>
+      </c>
+      <c r="L686" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Huevos</t>
+        </is>
+      </c>
+      <c r="C687" t="n">
+        <v>12</v>
+      </c>
+      <c r="D687" t="n">
+        <v>40</v>
+      </c>
+      <c r="E687" t="n">
+        <v>480</v>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H687" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I687" t="n">
+        <v>40</v>
+      </c>
+      <c r="J687" t="n">
+        <v>480</v>
+      </c>
+      <c r="K687" t="n">
+        <v>12</v>
+      </c>
+      <c r="L687" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Oferta</t>
+        </is>
+      </c>
+      <c r="C688" t="n">
+        <v>1</v>
+      </c>
+      <c r="D688" t="n">
+        <v>0</v>
+      </c>
+      <c r="E688" t="n">
+        <v>0</v>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H688" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I688" t="n">
+        <v>0</v>
+      </c>
+      <c r="J688" t="n">
+        <v>0</v>
+      </c>
+      <c r="L688" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>04/05/2025</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Aceite</t>
+        </is>
+      </c>
+      <c r="C689" t="n">
+        <v>20</v>
+      </c>
+      <c r="D689" t="n">
+        <v>200</v>
+      </c>
+      <c r="E689" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A.</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I689" t="n">
+        <v>200</v>
+      </c>
+      <c r="J689" t="n">
+        <v>4000</v>
+      </c>
+      <c r="K689" t="n">
+        <v>20</v>
+      </c>
+      <c r="L689" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Levadura Prensada Virgen Calsa Pan x 500 Gr</t>
+        </is>
+      </c>
+      <c r="C690" t="n">
+        <v>2</v>
+      </c>
+      <c r="D690" t="n">
+        <v>3537.26</v>
+      </c>
+      <c r="E690" t="n">
+        <v>7074.52</v>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H690" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I690" t="n">
+        <v>3537.26</v>
+      </c>
+      <c r="J690" t="n">
+        <v>7074.52</v>
+      </c>
+      <c r="K690" t="n">
+        <v>2</v>
+      </c>
+      <c r="L690" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Jamón Cocido Tradicional Campo Austral Pieza x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C691" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="D691" t="n">
+        <v>10371.05</v>
+      </c>
+      <c r="E691" t="n">
+        <v>51025.57</v>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I691" t="n">
+        <v>10364.73</v>
+      </c>
+      <c r="J691" t="n">
+        <v>50994.47</v>
+      </c>
+      <c r="K691" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="L691" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Queso Cheddar Fundido Milkaut Caja (2 x 3.5 Kg)</t>
+        </is>
+      </c>
+      <c r="C692" t="n">
+        <v>1</v>
+      </c>
+      <c r="D692" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="E692" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H692" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I692" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="J692" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="K692" t="n">
+        <v>1</v>
+      </c>
+      <c r="L692" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Queso Criña Milkaut Balde x 3.6 Kg</t>
+        </is>
+      </c>
+      <c r="C693" t="n">
+        <v>1</v>
+      </c>
+      <c r="D693" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="E693" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H693" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I693" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="J693" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="K693" t="n">
+        <v>1</v>
+      </c>
+      <c r="L693" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Panceta Ahumada Campo Austral Pieza x 2.2 Kg Aprox</t>
+        </is>
+      </c>
+      <c r="C694" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D694" t="n">
+        <v>135.22</v>
+      </c>
+      <c r="E694" t="n">
+        <v>155635.38</v>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H694" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I694" t="n">
+        <v>13527.63</v>
+      </c>
+      <c r="J694" t="n">
+        <v>15570302.13</v>
+      </c>
+      <c r="K694" t="n">
+        <v>1150.98</v>
+      </c>
+      <c r="L694" t="inlineStr">
+        <is>
+          <t>Q no</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Pan Rallado Preferido Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C695" t="n">
+        <v>2</v>
+      </c>
+      <c r="D695" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E695" t="n">
+        <v>17922.1</v>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I695" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J695" t="n">
+        <v>17922.1</v>
+      </c>
+      <c r="K695" t="n">
+        <v>2</v>
+      </c>
+      <c r="L695" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Galletitas Chocolipas Bagley Caja (25 x 250 Grs)</t>
+        </is>
+      </c>
+      <c r="C696" t="n">
+        <v>1</v>
+      </c>
+      <c r="D696" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="E696" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I696" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="J696" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="K696" t="n">
+        <v>1</v>
+      </c>
+      <c r="L696" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Cafe Soluble Arlistan Pack (12 x 170 Grs)</t>
+        </is>
+      </c>
+      <c r="C697" t="n">
+        <v>1</v>
+      </c>
+      <c r="D697" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="E697" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I697" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="J697" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="K697" t="n">
+        <v>1</v>
+      </c>
+      <c r="L697" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Tomate Perita Cumana Lata x 2.93 Kg</t>
+        </is>
+      </c>
+      <c r="C698" t="n">
+        <v>6</v>
+      </c>
+      <c r="D698" t="n">
+        <v>6387.35</v>
+      </c>
+      <c r="E698" t="n">
+        <v>38324.1</v>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I698" t="n">
+        <v>6387.35</v>
+      </c>
+      <c r="J698" t="n">
+        <v>38324.1</v>
+      </c>
+      <c r="K698" t="n">
+        <v>6</v>
+      </c>
+      <c r="L698" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Hanna de Trigo 0000 Cañuelas Bolsa x 25 Kg</t>
+        </is>
+      </c>
+      <c r="C699" t="n">
+        <v>2</v>
+      </c>
+      <c r="D699" t="n">
+        <v>16376.6</v>
+      </c>
+      <c r="E699" t="n">
+        <v>32753.2</v>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I699" t="n">
+        <v>16376.6</v>
+      </c>
+      <c r="J699" t="n">
+        <v>32753.2</v>
+      </c>
+      <c r="K699" t="n">
+        <v>2</v>
+      </c>
+      <c r="L699" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Fideos Spaghetti Nº7 Lucchetti Paquete (20 x 300 Grs)</t>
+        </is>
+      </c>
+      <c r="C700" t="n">
+        <v>1</v>
+      </c>
+      <c r="D700" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="E700" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I700" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="J700" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="K700" t="n">
+        <v>1</v>
+      </c>
+      <c r="L700" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Sal Fina Dos Anclas Paquete (12 x 500 Grs)</t>
+        </is>
+      </c>
+      <c r="C701" t="n">
+        <v>1</v>
+      </c>
+      <c r="D701" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="E701" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I701" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="J701" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="K701" t="n">
+        <v>1</v>
+      </c>
+      <c r="L701" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Caldo de Verdura Granulado Knorr Caja (6 x 650 Grs)</t>
+        </is>
+      </c>
+      <c r="C702" t="n">
+        <v>1</v>
+      </c>
+      <c r="D702" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="E702" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I702" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="J702" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="K702" t="n">
+        <v>1</v>
+      </c>
+      <c r="L702" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Aceite Alto Oleico Vero Caja (2 x 10 Lts)</t>
+        </is>
+      </c>
+      <c r="C703" t="n">
+        <v>3</v>
+      </c>
+      <c r="D703" t="n">
+        <v>62032.32</v>
+      </c>
+      <c r="E703" t="n">
+        <v>186096.96</v>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I703" t="n">
+        <v>62032.32</v>
+      </c>
+      <c r="J703" t="n">
+        <v>186096.96</v>
+      </c>
+      <c r="K703" t="n">
+        <v>3</v>
+      </c>
+      <c r="L703" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Salsa Demi Glace Safra Bolsa x 480 Grs</t>
+        </is>
+      </c>
+      <c r="C704" t="n">
+        <v>2</v>
+      </c>
+      <c r="D704" t="n">
+        <v>7795.79</v>
+      </c>
+      <c r="E704" t="n">
+        <v>15591.58</v>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I704" t="n">
+        <v>7795.79</v>
+      </c>
+      <c r="J704" t="n">
+        <v>15591.58</v>
+      </c>
+      <c r="K704" t="n">
+        <v>2</v>
+      </c>
+      <c r="L704" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Nueces Mariposas Extra Light Cumana Bolsa x 1 Kg</t>
+        </is>
+      </c>
+      <c r="C705" t="n">
+        <v>1</v>
+      </c>
+      <c r="D705" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="E705" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I705" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="J705" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="K705" t="n">
+        <v>1</v>
+      </c>
+      <c r="L705" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Papa McCain Tradicional (6 x 2.5 Kg) (A11109)x</t>
+        </is>
+      </c>
+      <c r="C706" t="n">
+        <v>8</v>
+      </c>
+      <c r="D706" t="n">
+        <v>32902.53</v>
+      </c>
+      <c r="E706" t="n">
+        <v>263220.24</v>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I706" t="n">
+        <v>32902.53</v>
+      </c>
+      <c r="J706" t="n">
+        <v>263220.24</v>
+      </c>
+      <c r="K706" t="n">
+        <v>8</v>
+      </c>
+      <c r="L706" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Chocolate Blanco Cobertura (90) Fenix Bolsa x 2.5 Kg</t>
+        </is>
+      </c>
+      <c r="C707" t="n">
+        <v>1</v>
+      </c>
+      <c r="D707" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="E707" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I707" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="J707" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="K707" t="n">
+        <v>1</v>
+      </c>
+      <c r="L707" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Pan Rallado Prefendo Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C708" t="n">
+        <v>1</v>
+      </c>
+      <c r="D708" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E708" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I708" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J708" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="K708" t="n">
+        <v>1</v>
+      </c>
+      <c r="L708" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Chip de Chocolate Semiamargo (9641) Aguila Caja x 10 Kg</t>
+        </is>
+      </c>
+      <c r="C709" t="n">
+        <v>1</v>
+      </c>
+      <c r="D709" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="E709" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I709" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="J709" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="K709" t="n">
+        <v>1</v>
+      </c>
+      <c r="L709" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Té Clásico Green Hills con sobre Pack (10 x 50 un)</t>
+        </is>
+      </c>
+      <c r="C710" t="n">
+        <v>18818.27</v>
+      </c>
+      <c r="D710" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="E710" t="n">
+        <v>140007.93</v>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>GRATTINADO</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I710" t="n">
+        <v>0</v>
+      </c>
+      <c r="J710" t="n">
+        <v>0</v>
+      </c>
+      <c r="K710" t="n">
+        <v>18818.27</v>
+      </c>
+      <c r="L710" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="J711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="K711" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Barritas de submarino Aguila Caja (24 x 14 gr)</t>
+        </is>
+      </c>
+      <c r="C712" t="n">
+        <v>1</v>
+      </c>
+      <c r="D712" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="E712" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I712" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="J712" t="n">
+        <v>14946.31</v>
+      </c>
+      <c r="K712" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Queso Crema Milka ut Balde x 3.6 Kg</t>
+        </is>
+      </c>
+      <c r="C713" t="n">
+        <v>2</v>
+      </c>
+      <c r="D713" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="E713" t="n">
+        <v>81397.06</v>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I713" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="J713" t="n">
+        <v>81397.06</v>
+      </c>
+      <c r="K713" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Rebozador Preferido Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C714" t="n">
+        <v>1</v>
+      </c>
+      <c r="D714" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E714" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I714" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J714" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="K714" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Levadura Prensada Virgen Calsa Pan x 500 Gr</t>
+        </is>
+      </c>
+      <c r="C715" t="n">
+        <v>2</v>
+      </c>
+      <c r="D715" t="n">
+        <v>3537.26</v>
+      </c>
+      <c r="E715" t="n">
+        <v>7074.52</v>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I715" t="n">
+        <v>3537.26</v>
+      </c>
+      <c r="J715" t="n">
+        <v>7074.52</v>
+      </c>
+      <c r="K715" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Jamón Cocido Tradicional Campo Austral Pieza x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C716" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="D716" t="n">
+        <v>10371.05</v>
+      </c>
+      <c r="E716" t="n">
+        <v>51025.57</v>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I716" t="n">
+        <v>10364.73</v>
+      </c>
+      <c r="J716" t="n">
+        <v>50994.47</v>
+      </c>
+      <c r="K716" t="n">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Queso Cheddar Fundido Milkaut Caja (2 x 3.5 Kg)</t>
+        </is>
+      </c>
+      <c r="C717" t="n">
+        <v>1</v>
+      </c>
+      <c r="D717" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="E717" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I717" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="J717" t="n">
+        <v>59358.44</v>
+      </c>
+      <c r="K717" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Queso Criña Milkaut Balde x 3.6 Kg</t>
+        </is>
+      </c>
+      <c r="C718" t="n">
+        <v>1</v>
+      </c>
+      <c r="D718" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="E718" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I718" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="J718" t="n">
+        <v>40698.53</v>
+      </c>
+      <c r="K718" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Panceta Ahumada Campo Austral Pieza x 2.2 Kg Aprox</t>
+        </is>
+      </c>
+      <c r="C719" t="n">
+        <v>11.51</v>
+      </c>
+      <c r="D719" t="n">
+        <v>13521.75</v>
+      </c>
+      <c r="E719" t="n">
+        <v>155635.38</v>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H719" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I719" t="n">
+        <v>13527.63</v>
+      </c>
+      <c r="J719" t="n">
+        <v>155703.02</v>
+      </c>
+      <c r="K719" t="n">
+        <v>11.51</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Pan Rallado Preferido Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C720" t="n">
+        <v>2</v>
+      </c>
+      <c r="D720" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E720" t="n">
+        <v>17922.1</v>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H720" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I720" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J720" t="n">
+        <v>17922.1</v>
+      </c>
+      <c r="K720" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Galletitas Chocolipas Bagley Caja (25 x 250 Grs)</t>
+        </is>
+      </c>
+      <c r="C721" t="n">
+        <v>1</v>
+      </c>
+      <c r="D721" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="E721" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H721" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I721" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="J721" t="n">
+        <v>37120.66</v>
+      </c>
+      <c r="K721" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Cafe Soluble Arlistan Pack (12 x 170 Grs)</t>
+        </is>
+      </c>
+      <c r="C722" t="n">
+        <v>1</v>
+      </c>
+      <c r="D722" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="E722" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H722" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I722" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="J722" t="n">
+        <v>62188.07</v>
+      </c>
+      <c r="K722" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Tomate Perita Cumana Lata x 2.93 Kg</t>
+        </is>
+      </c>
+      <c r="C723" t="n">
+        <v>6</v>
+      </c>
+      <c r="D723" t="n">
+        <v>6387.35</v>
+      </c>
+      <c r="E723" t="n">
+        <v>38324.1</v>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H723" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I723" t="n">
+        <v>6387.35</v>
+      </c>
+      <c r="J723" t="n">
+        <v>38324.1</v>
+      </c>
+      <c r="K723" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Hanna de Trigo 0000 Cañuelas Bolsa x 25 Kg</t>
+        </is>
+      </c>
+      <c r="C724" t="n">
+        <v>2</v>
+      </c>
+      <c r="D724" t="n">
+        <v>16376.6</v>
+      </c>
+      <c r="E724" t="n">
+        <v>32753.2</v>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H724" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I724" t="n">
+        <v>16376.6</v>
+      </c>
+      <c r="J724" t="n">
+        <v>32753.2</v>
+      </c>
+      <c r="K724" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Fideos Spaghetti Nº7 Lucchetti Paquete (20 x 300 Grs)</t>
+        </is>
+      </c>
+      <c r="C725" t="n">
+        <v>1</v>
+      </c>
+      <c r="D725" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="E725" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H725" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I725" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="J725" t="n">
+        <v>18010.62</v>
+      </c>
+      <c r="K725" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Sal Fina Dos Anclas Paquete (12 x 500 Grs)</t>
+        </is>
+      </c>
+      <c r="C726" t="n">
+        <v>1</v>
+      </c>
+      <c r="D726" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="E726" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H726" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I726" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="J726" t="n">
+        <v>11113.6</v>
+      </c>
+      <c r="K726" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Caldo de Verdura Granulado Knorr Caja (6 x 650 Grs)</t>
+        </is>
+      </c>
+      <c r="C727" t="n">
+        <v>1</v>
+      </c>
+      <c r="D727" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="E727" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H727" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I727" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="J727" t="n">
+        <v>57980.3</v>
+      </c>
+      <c r="K727" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Aceite Alto Oleico Vero Caja (2 x 10 Lts)</t>
+        </is>
+      </c>
+      <c r="C728" t="n">
+        <v>3</v>
+      </c>
+      <c r="D728" t="n">
+        <v>62032.32</v>
+      </c>
+      <c r="E728" t="n">
+        <v>186096.96</v>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H728" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I728" t="n">
+        <v>62032.32</v>
+      </c>
+      <c r="J728" t="n">
+        <v>186096.96</v>
+      </c>
+      <c r="K728" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Salsa Demi Glace Safra Bolsa x 480 Grs</t>
+        </is>
+      </c>
+      <c r="C729" t="n">
+        <v>2</v>
+      </c>
+      <c r="D729" t="n">
+        <v>7795.79</v>
+      </c>
+      <c r="E729" t="n">
+        <v>15591.58</v>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H729" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I729" t="n">
+        <v>7795.79</v>
+      </c>
+      <c r="J729" t="n">
+        <v>15591.58</v>
+      </c>
+      <c r="K729" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Nueces Mariposas Extra Light Cumana Bolsa x 1 Kg</t>
+        </is>
+      </c>
+      <c r="C730" t="n">
+        <v>1</v>
+      </c>
+      <c r="D730" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="E730" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H730" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I730" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="J730" t="n">
+        <v>21573.3</v>
+      </c>
+      <c r="K730" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Papa McCain Tradicional (6 x 2.5 Kg) (A11109)x</t>
+        </is>
+      </c>
+      <c r="C731" t="n">
+        <v>8</v>
+      </c>
+      <c r="D731" t="n">
+        <v>32902.53</v>
+      </c>
+      <c r="E731" t="n">
+        <v>263220.24</v>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>Rissolar Pilar S.A.</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H731" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I731" t="n">
+        <v>32902.53</v>
+      </c>
+      <c r="J731" t="n">
+        <v>263220.24</v>
+      </c>
+      <c r="K731" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Chocolate Blanco Cobertura (90) Fenix Bolsa x 2.5 Kg</t>
+        </is>
+      </c>
+      <c r="C732" t="n">
+        <v>1</v>
+      </c>
+      <c r="D732" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="E732" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H732" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I732" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="J732" t="n">
+        <v>65912.17999999999</v>
+      </c>
+      <c r="K732" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Pan Rallado Prefendo Bolsa x 5 Kg</t>
+        </is>
+      </c>
+      <c r="C733" t="n">
+        <v>1</v>
+      </c>
+      <c r="D733" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="E733" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H733" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I733" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="J733" t="n">
+        <v>8961.049999999999</v>
+      </c>
+      <c r="K733" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Chip de Chocolate Semiamargo (9641) Aguila Caja x 10 Kg</t>
+        </is>
+      </c>
+      <c r="C734" t="n">
+        <v>1</v>
+      </c>
+      <c r="D734" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="E734" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>Mojama SA</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H734" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I734" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="J734" t="n">
+        <v>56017.25</v>
+      </c>
+      <c r="K734" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Té Clásico Green Hills con sobre Pack (10 x 50 un)</t>
+        </is>
+      </c>
+      <c r="C735" t="n">
+        <v>0</v>
+      </c>
+      <c r="D735" t="n">
+        <v>0</v>
+      </c>
+      <c r="E735" t="n">
+        <v>0</v>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>GRATTINADO</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>Mayorista Net</t>
+        </is>
+      </c>
+      <c r="H735" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I735" t="n">
+        <v>0</v>
+      </c>
+      <c r="J735" t="n">
+        <v>0</v>
+      </c>
+      <c r="K735" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document AI - Quilmes OK
</commit_message>
<xml_diff>
--- a/BD extracciones.xlsx
+++ b/BD extracciones.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S460"/>
+  <dimension ref="A1:S468"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23575,6 +23575,246 @@
       </c>
       <c r="P460" t="n">
         <v>4108.61</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr"/>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="inlineStr"/>
+      <c r="D461" t="inlineStr"/>
+      <c r="E461" t="inlineStr"/>
+      <c r="F461" t="inlineStr"/>
+      <c r="G461" t="inlineStr"/>
+      <c r="H461" t="inlineStr"/>
+      <c r="I461" t="inlineStr"/>
+      <c r="J461" t="inlineStr"/>
+      <c r="K461" t="inlineStr"/>
+      <c r="L461" t="n">
+        <v>14933</v>
+      </c>
+      <c r="M461" t="inlineStr">
+        <is>
+          <t>ECO AND S/GAS 500x12 PET</t>
+        </is>
+      </c>
+      <c r="N461" t="n">
+        <v>1</v>
+      </c>
+      <c r="O461" t="n">
+        <v>16590.12</v>
+      </c>
+      <c r="P461" t="n">
+        <v>280572.11</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr"/>
+      <c r="B462" t="inlineStr"/>
+      <c r="C462" t="inlineStr"/>
+      <c r="D462" t="inlineStr"/>
+      <c r="E462" t="inlineStr"/>
+      <c r="F462" t="inlineStr"/>
+      <c r="G462" t="inlineStr"/>
+      <c r="H462" t="inlineStr"/>
+      <c r="I462" t="inlineStr"/>
+      <c r="J462" t="inlineStr"/>
+      <c r="K462" t="inlineStr"/>
+      <c r="L462" t="n">
+        <v>30481</v>
+      </c>
+      <c r="M462" t="inlineStr">
+        <is>
+          <t>SEVEN-UP NF CAN 130 BUL/PAL 4X6</t>
+        </is>
+      </c>
+      <c r="N462" t="n">
+        <v>1</v>
+      </c>
+      <c r="O462" t="n">
+        <v>45123.14</v>
+      </c>
+      <c r="P462" t="n">
+        <v>36098.51</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr"/>
+      <c r="B463" t="inlineStr"/>
+      <c r="C463" t="inlineStr"/>
+      <c r="D463" t="inlineStr"/>
+      <c r="E463" t="inlineStr"/>
+      <c r="F463" t="inlineStr"/>
+      <c r="G463" t="inlineStr"/>
+      <c r="H463" t="inlineStr"/>
+      <c r="I463" t="inlineStr"/>
+      <c r="J463" t="inlineStr"/>
+      <c r="K463" t="inlineStr"/>
+      <c r="L463" t="n">
+        <v>30648</v>
+      </c>
+      <c r="M463" t="inlineStr">
+        <is>
+          <t>PEPSI CAN 4X6 354CC TITAN</t>
+        </is>
+      </c>
+      <c r="N463" t="n">
+        <v>1</v>
+      </c>
+      <c r="O463" t="n">
+        <v>24297.16</v>
+      </c>
+      <c r="P463" t="n">
+        <v>12148.58</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr"/>
+      <c r="B464" t="inlineStr"/>
+      <c r="C464" t="inlineStr"/>
+      <c r="D464" t="inlineStr"/>
+      <c r="E464" t="inlineStr"/>
+      <c r="F464" t="inlineStr"/>
+      <c r="G464" t="inlineStr"/>
+      <c r="H464" t="inlineStr"/>
+      <c r="I464" t="inlineStr"/>
+      <c r="J464" t="inlineStr"/>
+      <c r="K464" t="inlineStr"/>
+      <c r="L464" t="n">
+        <v>31205</v>
+      </c>
+      <c r="M464" t="inlineStr">
+        <is>
+          <t>ANDES ORIGEN RUBIA 2.0 CAN 4X6</t>
+        </is>
+      </c>
+      <c r="N464" t="n">
+        <v>1</v>
+      </c>
+      <c r="O464" t="n">
+        <v>23448.54</v>
+      </c>
+      <c r="P464" t="n">
+        <v>11724.27</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr"/>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="inlineStr"/>
+      <c r="D465" t="inlineStr"/>
+      <c r="E465" t="inlineStr"/>
+      <c r="F465" t="inlineStr"/>
+      <c r="G465" t="inlineStr"/>
+      <c r="H465" t="inlineStr"/>
+      <c r="I465" t="inlineStr"/>
+      <c r="J465" t="inlineStr"/>
+      <c r="K465" t="inlineStr"/>
+      <c r="L465" t="n">
+        <v>30793</v>
+      </c>
+      <c r="M465" t="inlineStr">
+        <is>
+          <t>PEPSI BLACK CAN 4X6 354CC TITAN</t>
+        </is>
+      </c>
+      <c r="N465" t="n">
+        <v>3</v>
+      </c>
+      <c r="O465" t="n">
+        <v>23448.54</v>
+      </c>
+      <c r="P465" t="n">
+        <v>11724.27</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr"/>
+      <c r="B466" t="inlineStr"/>
+      <c r="C466" t="inlineStr"/>
+      <c r="D466" t="inlineStr"/>
+      <c r="E466" t="inlineStr"/>
+      <c r="F466" t="inlineStr"/>
+      <c r="G466" t="inlineStr"/>
+      <c r="H466" t="inlineStr"/>
+      <c r="I466" t="inlineStr"/>
+      <c r="J466" t="inlineStr"/>
+      <c r="K466" t="inlineStr"/>
+      <c r="L466" t="n">
+        <v>28317</v>
+      </c>
+      <c r="M466" t="inlineStr">
+        <is>
+          <t>CORONA OW X24 330CC</t>
+        </is>
+      </c>
+      <c r="N466" t="n">
+        <v>1</v>
+      </c>
+      <c r="O466" t="n">
+        <v>58648.38</v>
+      </c>
+      <c r="P466" t="n">
+        <v>123161.6</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr"/>
+      <c r="B467" t="inlineStr"/>
+      <c r="C467" t="inlineStr"/>
+      <c r="D467" t="inlineStr"/>
+      <c r="E467" t="inlineStr"/>
+      <c r="F467" t="inlineStr"/>
+      <c r="G467" t="inlineStr"/>
+      <c r="H467" t="inlineStr"/>
+      <c r="I467" t="inlineStr"/>
+      <c r="J467" t="inlineStr"/>
+      <c r="K467" t="inlineStr"/>
+      <c r="L467" t="n">
+        <v>31074</v>
+      </c>
+      <c r="M467" t="inlineStr">
+        <is>
+          <t>PDT POMELO CAN 4X6 269CC 169 BU</t>
+        </is>
+      </c>
+      <c r="N467" t="n">
+        <v>1</v>
+      </c>
+      <c r="O467" t="n">
+        <v>19219.67</v>
+      </c>
+      <c r="P467" t="n">
+        <v>9609.82</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr"/>
+      <c r="B468" t="inlineStr"/>
+      <c r="C468" t="inlineStr"/>
+      <c r="D468" t="inlineStr"/>
+      <c r="E468" t="inlineStr"/>
+      <c r="F468" t="inlineStr"/>
+      <c r="G468" t="inlineStr"/>
+      <c r="H468" t="inlineStr"/>
+      <c r="I468" t="inlineStr"/>
+      <c r="J468" t="inlineStr"/>
+      <c r="K468" t="inlineStr"/>
+      <c r="L468" t="n">
+        <v>99900</v>
+      </c>
+      <c r="M468" t="inlineStr">
+        <is>
+          <t>SERVICIO LOGISTICO</t>
+        </is>
+      </c>
+      <c r="N468" t="n">
+        <v>1</v>
+      </c>
+      <c r="O468" t="n">
+        <v>3660</v>
+      </c>
+      <c r="P468" t="n">
+        <v>3660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entre amigos ok, testear
</commit_message>
<xml_diff>
--- a/BD extracciones.xlsx
+++ b/BD extracciones.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -854,6 +854,975 @@
         <v>16126.24</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>214</v>
+      </c>
+      <c r="D7" t="n">
+        <v>330</v>
+      </c>
+      <c r="E7" t="n">
+        <v>70620</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>COSTA 7070</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J7" t="n">
+        <v>706200</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="N7" t="n">
+        <v>3300</v>
+      </c>
+      <c r="O7" t="n">
+        <v>70620</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>116</v>
+      </c>
+      <c r="D8" t="n">
+        <v>838</v>
+      </c>
+      <c r="E8" t="n">
+        <v>97208</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J8" t="n">
+        <v>972080</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O8" t="n">
+        <v>97208</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>95</v>
+      </c>
+      <c r="D9" t="n">
+        <v>838</v>
+      </c>
+      <c r="E9" t="n">
+        <v>79610</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J9" t="n">
+        <v>796100</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O9" t="n">
+        <v>79610</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>150</v>
+      </c>
+      <c r="D10" t="n">
+        <v>600</v>
+      </c>
+      <c r="E10" t="n">
+        <v>90000</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>900000</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>15</v>
+      </c>
+      <c r="N10" t="n">
+        <v>6000</v>
+      </c>
+      <c r="O10" t="n">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>150</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1193.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>179025</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>11935</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1790250</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>15</v>
+      </c>
+      <c r="N11" t="n">
+        <v>11935</v>
+      </c>
+      <c r="O11" t="n">
+        <v>179025</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E12" t="n">
+        <v>70620</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>COSTA 7070</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J12" t="n">
+        <v>70620</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="N12" t="n">
+        <v>3300</v>
+      </c>
+      <c r="O12" t="n">
+        <v>70620</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>116</v>
+      </c>
+      <c r="D13" t="n">
+        <v>838</v>
+      </c>
+      <c r="E13" t="n">
+        <v>97208</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J13" t="n">
+        <v>972080</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N13" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O13" t="n">
+        <v>97208</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>95</v>
+      </c>
+      <c r="D14" t="n">
+        <v>838</v>
+      </c>
+      <c r="E14" t="n">
+        <v>79610</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J14" t="n">
+        <v>796100</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N14" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O14" t="n">
+        <v>79610</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D15" t="n">
+        <v>600</v>
+      </c>
+      <c r="E15" t="n">
+        <v>90000</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J15" t="n">
+        <v>900000</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>15</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6000</v>
+      </c>
+      <c r="O15" t="n">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>150</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1193.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>179025</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>11935</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1790250</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>15</v>
+      </c>
+      <c r="N16" t="n">
+        <v>11935</v>
+      </c>
+      <c r="O16" t="n">
+        <v>179025</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E17" t="n">
+        <v>70620</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>COSTA 7070</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J17" t="n">
+        <v>70620</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="N17" t="n">
+        <v>3300</v>
+      </c>
+      <c r="O17" t="n">
+        <v>70620</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E18" t="n">
+        <v>70620</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>COSTA 7070</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J18" t="n">
+        <v>70620</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="N18" t="n">
+        <v>3300</v>
+      </c>
+      <c r="O18" t="n">
+        <v>70620</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="D19" t="n">
+        <v>8380</v>
+      </c>
+      <c r="E19" t="n">
+        <v>97208</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J19" t="n">
+        <v>97208</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N19" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O19" t="n">
+        <v>97208</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8380</v>
+      </c>
+      <c r="E20" t="n">
+        <v>79610</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J20" t="n">
+        <v>79610</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N20" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O20" t="n">
+        <v>79610</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>15</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E21" t="n">
+        <v>90000</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J21" t="n">
+        <v>90000</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>15</v>
+      </c>
+      <c r="N21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="O21" t="n">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>15</v>
+      </c>
+      <c r="D22" t="n">
+        <v>11935</v>
+      </c>
+      <c r="E22" t="n">
+        <v>179025</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>11935</v>
+      </c>
+      <c r="J22" t="n">
+        <v>179025</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>15</v>
+      </c>
+      <c r="N22" t="n">
+        <v>11935</v>
+      </c>
+      <c r="O22" t="n">
+        <v>179025</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E23" t="n">
+        <v>70620</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>COSTA 7070</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J23" t="n">
+        <v>70620</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>PATA Y MUSLO</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="N23" t="n">
+        <v>3300</v>
+      </c>
+      <c r="O23" t="n">
+        <v>70620</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Pereira ok, entre amigos mistral puede fallar gem ok, avez mistral puede fallar gem ok, criollo ok
</commit_message>
<xml_diff>
--- a/BD extracciones.xlsx
+++ b/BD extracciones.xlsx
@@ -436,11 +436,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -459,8 +459,8 @@
     <col width="6.77734375" bestFit="1" customWidth="1" style="4" min="13" max="13"/>
     <col width="11" bestFit="1" customWidth="1" style="4" min="14" max="14"/>
     <col width="11.21875" bestFit="1" customWidth="1" style="4" min="15" max="15"/>
-    <col width="5.21875" bestFit="1" customWidth="1" style="10" min="16" max="16"/>
-    <col width="9.5546875" bestFit="1" customWidth="1" style="10" min="17" max="17"/>
+    <col width="9.21875" bestFit="1" customWidth="1" style="10" min="16" max="16"/>
+    <col width="9.33203125" bestFit="1" customWidth="1" style="10" min="17" max="17"/>
     <col width="11.109375" bestFit="1" customWidth="1" style="10" min="18" max="18"/>
     <col width="11.5546875" bestFit="1" customWidth="1" min="20" max="20"/>
   </cols>
@@ -682,6 +682,18 @@
       <c r="O3" t="n">
         <v>20520.94</v>
       </c>
+      <c r="P3" s="9">
+        <f>+C3-M3</f>
+        <v/>
+      </c>
+      <c r="Q3" s="9">
+        <f>+D3-N3</f>
+        <v/>
+      </c>
+      <c r="R3" s="9">
+        <f>+E3-O3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -739,6 +751,18 @@
       <c r="O4" t="n">
         <v>16126.24</v>
       </c>
+      <c r="P4" s="9">
+        <f>+C4-M4</f>
+        <v/>
+      </c>
+      <c r="Q4" s="9">
+        <f>+D4-N4</f>
+        <v/>
+      </c>
+      <c r="R4" s="9">
+        <f>+E4-O4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -796,6 +820,18 @@
       <c r="O5" t="n">
         <v>16126.24</v>
       </c>
+      <c r="P5" s="9">
+        <f>+C5-M5</f>
+        <v/>
+      </c>
+      <c r="Q5" s="9">
+        <f>+D5-N5</f>
+        <v/>
+      </c>
+      <c r="R5" s="9">
+        <f>+E5-O5</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -853,6 +889,18 @@
       <c r="O6" t="n">
         <v>16126.24</v>
       </c>
+      <c r="P6" s="9">
+        <f>+C6-M6</f>
+        <v/>
+      </c>
+      <c r="Q6" s="9">
+        <f>+D6-N6</f>
+        <v/>
+      </c>
+      <c r="R6" s="9">
+        <f>+E6-O6</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -910,6 +958,18 @@
       <c r="O7" t="n">
         <v>70620</v>
       </c>
+      <c r="P7" s="9">
+        <f>+C7-M7</f>
+        <v/>
+      </c>
+      <c r="Q7" s="9">
+        <f>+D7-N7</f>
+        <v/>
+      </c>
+      <c r="R7" s="9">
+        <f>+E7-O7</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -967,6 +1027,18 @@
       <c r="O8" t="n">
         <v>97208</v>
       </c>
+      <c r="P8" s="9">
+        <f>+C8-M8</f>
+        <v/>
+      </c>
+      <c r="Q8" s="9">
+        <f>+D8-N8</f>
+        <v/>
+      </c>
+      <c r="R8" s="9">
+        <f>+E8-O8</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1024,6 +1096,18 @@
       <c r="O9" t="n">
         <v>79610</v>
       </c>
+      <c r="P9" s="9">
+        <f>+C9-M9</f>
+        <v/>
+      </c>
+      <c r="Q9" s="9">
+        <f>+D9-N9</f>
+        <v/>
+      </c>
+      <c r="R9" s="9">
+        <f>+E9-O9</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1081,6 +1165,18 @@
       <c r="O10" t="n">
         <v>90000</v>
       </c>
+      <c r="P10" s="9">
+        <f>+C10-M10</f>
+        <v/>
+      </c>
+      <c r="Q10" s="9">
+        <f>+D10-N10</f>
+        <v/>
+      </c>
+      <c r="R10" s="9">
+        <f>+E10-O10</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1138,6 +1234,18 @@
       <c r="O11" t="n">
         <v>179025</v>
       </c>
+      <c r="P11" s="9">
+        <f>+C11-M11</f>
+        <v/>
+      </c>
+      <c r="Q11" s="9">
+        <f>+D11-N11</f>
+        <v/>
+      </c>
+      <c r="R11" s="9">
+        <f>+E11-O11</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1195,6 +1303,18 @@
       <c r="O12" t="n">
         <v>70620</v>
       </c>
+      <c r="P12" s="9">
+        <f>+C12-M12</f>
+        <v/>
+      </c>
+      <c r="Q12" s="9">
+        <f>+D12-N12</f>
+        <v/>
+      </c>
+      <c r="R12" s="9">
+        <f>+E12-O12</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1252,6 +1372,18 @@
       <c r="O13" t="n">
         <v>97208</v>
       </c>
+      <c r="P13" s="9">
+        <f>+C13-M13</f>
+        <v/>
+      </c>
+      <c r="Q13" s="9">
+        <f>+D13-N13</f>
+        <v/>
+      </c>
+      <c r="R13" s="9">
+        <f>+E13-O13</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1309,6 +1441,18 @@
       <c r="O14" t="n">
         <v>79610</v>
       </c>
+      <c r="P14" s="9">
+        <f>+C14-M14</f>
+        <v/>
+      </c>
+      <c r="Q14" s="9">
+        <f>+D14-N14</f>
+        <v/>
+      </c>
+      <c r="R14" s="9">
+        <f>+E14-O14</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1366,6 +1510,18 @@
       <c r="O15" t="n">
         <v>90000</v>
       </c>
+      <c r="P15" s="9">
+        <f>+C15-M15</f>
+        <v/>
+      </c>
+      <c r="Q15" s="9">
+        <f>+D15-N15</f>
+        <v/>
+      </c>
+      <c r="R15" s="9">
+        <f>+E15-O15</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1423,6 +1579,18 @@
       <c r="O16" t="n">
         <v>179025</v>
       </c>
+      <c r="P16" s="9">
+        <f>+C16-M16</f>
+        <v/>
+      </c>
+      <c r="Q16" s="9">
+        <f>+D16-N16</f>
+        <v/>
+      </c>
+      <c r="R16" s="9">
+        <f>+E16-O16</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1480,6 +1648,18 @@
       <c r="O17" t="n">
         <v>70620</v>
       </c>
+      <c r="P17" s="9">
+        <f>+C17-M17</f>
+        <v/>
+      </c>
+      <c r="Q17" s="9">
+        <f>+D17-N17</f>
+        <v/>
+      </c>
+      <c r="R17" s="9">
+        <f>+E17-O17</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1537,6 +1717,18 @@
       <c r="O18" t="n">
         <v>70620</v>
       </c>
+      <c r="P18" s="9">
+        <f>+C18-M18</f>
+        <v/>
+      </c>
+      <c r="Q18" s="9">
+        <f>+D18-N18</f>
+        <v/>
+      </c>
+      <c r="R18" s="9">
+        <f>+E18-O18</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1594,6 +1786,18 @@
       <c r="O19" t="n">
         <v>97208</v>
       </c>
+      <c r="P19" s="9">
+        <f>+C19-M19</f>
+        <v/>
+      </c>
+      <c r="Q19" s="9">
+        <f>+D19-N19</f>
+        <v/>
+      </c>
+      <c r="R19" s="9">
+        <f>+E19-O19</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1651,6 +1855,18 @@
       <c r="O20" t="n">
         <v>79610</v>
       </c>
+      <c r="P20" s="9">
+        <f>+C20-M20</f>
+        <v/>
+      </c>
+      <c r="Q20" s="9">
+        <f>+D20-N20</f>
+        <v/>
+      </c>
+      <c r="R20" s="9">
+        <f>+E20-O20</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1708,6 +1924,18 @@
       <c r="O21" t="n">
         <v>90000</v>
       </c>
+      <c r="P21" s="9">
+        <f>+C21-M21</f>
+        <v/>
+      </c>
+      <c r="Q21" s="9">
+        <f>+D21-N21</f>
+        <v/>
+      </c>
+      <c r="R21" s="9">
+        <f>+E21-O21</f>
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1765,6 +1993,18 @@
       <c r="O22" t="n">
         <v>179025</v>
       </c>
+      <c r="P22" s="9">
+        <f>+C22-M22</f>
+        <v/>
+      </c>
+      <c r="Q22" s="9">
+        <f>+D22-N22</f>
+        <v/>
+      </c>
+      <c r="R22" s="9">
+        <f>+E22-O22</f>
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1821,6 +2061,2190 @@
       </c>
       <c r="O23" t="n">
         <v>70620</v>
+      </c>
+      <c r="P23" s="9">
+        <f>+C23-M23</f>
+        <v/>
+      </c>
+      <c r="Q23" s="9">
+        <f>+D23-N23</f>
+        <v/>
+      </c>
+      <c r="R23" s="9">
+        <f>+E23-O23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>240001</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT AZUL X 700</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>CRUZA RECOLETA</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>1075329</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1075329</v>
+      </c>
+      <c r="K24" t="n">
+        <v>240001</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT AZUL X 700</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N24" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="O24" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="P24" s="9">
+        <f>+C24-M24</f>
+        <v/>
+      </c>
+      <c r="Q24" s="9">
+        <f>+D24-N24</f>
+        <v/>
+      </c>
+      <c r="R24" s="9">
+        <f>+E24-O24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>240070</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT RASFBERRI 6 X 700</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="E25" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CRUZA RECOLETA</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>1191031</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1191031</v>
+      </c>
+      <c r="K25" t="n">
+        <v>240070</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT RASPBERRI 6 X 700</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N25" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="O25" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="P25" s="9">
+        <f>+C25-M25</f>
+        <v/>
+      </c>
+      <c r="Q25" s="9">
+        <f>+D25-N25</f>
+        <v/>
+      </c>
+      <c r="R25" s="9">
+        <f>+E25-O25</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>340027</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT ELYX X 1000</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>46747.23</v>
+      </c>
+      <c r="E26" t="n">
+        <v>46747.23</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>La Mala</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>4674723</v>
+      </c>
+      <c r="J26" t="n">
+        <v>4674723</v>
+      </c>
+      <c r="K26" t="n">
+        <v>340027</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT ELYX X 1000</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N26" t="n">
+        <v>46747.23</v>
+      </c>
+      <c r="O26" t="n">
+        <v>46747.23</v>
+      </c>
+      <c r="P26" s="9">
+        <f>+C26-M26</f>
+        <v/>
+      </c>
+      <c r="Q26" s="9">
+        <f>+D26-N26</f>
+        <v/>
+      </c>
+      <c r="R26" s="9">
+        <f>+E26-O26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>240021</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>VODKA GREY GOOSE X 750</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>38705.73</v>
+      </c>
+      <c r="E27" t="n">
+        <v>387057.28</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>La Mala</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>6450955</v>
+      </c>
+      <c r="J27" t="n">
+        <v>64509550</v>
+      </c>
+      <c r="K27" t="n">
+        <v>240021</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>VODKA GREY GOOSE X 750</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" t="n">
+        <v>64509.55</v>
+      </c>
+      <c r="O27" t="n">
+        <v>387057.28</v>
+      </c>
+      <c r="P27" s="9">
+        <f>+C27-M27</f>
+        <v/>
+      </c>
+      <c r="Q27" s="9">
+        <f>+D27-N27</f>
+        <v/>
+      </c>
+      <c r="R27" s="9">
+        <f>+E27-O27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>240014</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>VODKA BELVEDERE X 700</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>53070.66</v>
+      </c>
+      <c r="E28" t="n">
+        <v>106141.32</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>La Mala</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>5307066</v>
+      </c>
+      <c r="J28" t="n">
+        <v>10614132</v>
+      </c>
+      <c r="K28" t="n">
+        <v>240014</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>VODKA BELVEDERE X 700</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="N28" t="n">
+        <v>53070.66</v>
+      </c>
+      <c r="O28" t="n">
+        <v>106141.32</v>
+      </c>
+      <c r="P28" s="9">
+        <f>+C28-M28</f>
+        <v/>
+      </c>
+      <c r="Q28" s="9">
+        <f>+D28-N28</f>
+        <v/>
+      </c>
+      <c r="R28" s="9">
+        <f>+E28-O28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>100022</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CH. VEUVE CLICQUOT BRUT X 750</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="n">
+        <v>121452.89</v>
+      </c>
+      <c r="E29" t="n">
+        <v>364358.68</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>La Mala</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>12145289</v>
+      </c>
+      <c r="J29" t="n">
+        <v>36435867</v>
+      </c>
+      <c r="K29" t="n">
+        <v>100022</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>CH. VEUVE CLICQUOT BRUT X 750</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N29" t="n">
+        <v>121452.89</v>
+      </c>
+      <c r="O29" t="n">
+        <v>364358.68</v>
+      </c>
+      <c r="P29" s="9">
+        <f>+C29-M29</f>
+        <v/>
+      </c>
+      <c r="Q29" s="9">
+        <f>+D29-N29</f>
+        <v/>
+      </c>
+      <c r="R29" s="9">
+        <f>+E29-O29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>190036</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>GIN TANQUERAY ENGLISH X 700</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>20</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8341.459999999999</v>
+      </c>
+      <c r="E30" t="n">
+        <v>166829.21</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>La Mala</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1390243</v>
+      </c>
+      <c r="J30" t="n">
+        <v>27804860</v>
+      </c>
+      <c r="K30" t="n">
+        <v>190036</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>GIN TANQUERAY ENGLISH X 700</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>2</v>
+      </c>
+      <c r="N30" t="n">
+        <v>13902.43</v>
+      </c>
+      <c r="O30" t="n">
+        <v>166829.21</v>
+      </c>
+      <c r="P30" s="9">
+        <f>+C30-M30</f>
+        <v/>
+      </c>
+      <c r="Q30" s="9">
+        <f>+D30-N30</f>
+        <v/>
+      </c>
+      <c r="R30" s="9">
+        <f>+E30-O30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>100001</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CH. BARON B B.NATURE X 750</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>40</v>
+      </c>
+      <c r="D31" t="n">
+        <v>14413.13</v>
+      </c>
+      <c r="E31" t="n">
+        <v>576525.39</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>2402189</v>
+      </c>
+      <c r="J31" t="n">
+        <v>96087560</v>
+      </c>
+      <c r="K31" t="n">
+        <v>100001</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>CH. BARON B B.NATURE X 750</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>4</v>
+      </c>
+      <c r="N31" t="n">
+        <v>24021.89</v>
+      </c>
+      <c r="O31" t="n">
+        <v>576525.39</v>
+      </c>
+      <c r="P31" s="9">
+        <f>+C31-M31</f>
+        <v/>
+      </c>
+      <c r="Q31" s="9">
+        <f>+D31-N31</f>
+        <v/>
+      </c>
+      <c r="R31" s="9">
+        <f>+E31-O31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>240001</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT AZUL X 700</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="E32" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>CRUZA RECOLETA</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>1075329</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1075329</v>
+      </c>
+      <c r="K32" t="n">
+        <v>240001</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT AZUL X 700</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>12</v>
+      </c>
+      <c r="N32" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="O32" t="n">
+        <v>10753.29</v>
+      </c>
+      <c r="P32" s="9">
+        <f>+C32-M32</f>
+        <v/>
+      </c>
+      <c r="Q32" s="9">
+        <f>+D32-N32</f>
+        <v/>
+      </c>
+      <c r="R32" s="9">
+        <f>+E32-O32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>240070</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT RASFBERRI 6 X 700</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="E33" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>CRUZA RECOLETA</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>1191031</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1191031</v>
+      </c>
+      <c r="K33" t="n">
+        <v>240070</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>VODKA ABSOLUT RASPBERRI 6 X 700</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>6</v>
+      </c>
+      <c r="N33" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="O33" t="n">
+        <v>11910.31</v>
+      </c>
+      <c r="P33" s="9">
+        <f>+C33-M33</f>
+        <v/>
+      </c>
+      <c r="Q33" s="9">
+        <f>+D33-N33</f>
+        <v/>
+      </c>
+      <c r="R33" s="9">
+        <f>+E33-O33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>OJO DE BIFE</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="D34" t="n">
+        <v>15535</v>
+      </c>
+      <c r="E34" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Galicia Polo Mince Bar</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>15535</v>
+      </c>
+      <c r="J34" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>OJO DE BIFE</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="N34" t="n">
+        <v>15535</v>
+      </c>
+      <c r="O34" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="P34" s="9">
+        <f>+C34-M34</f>
+        <v/>
+      </c>
+      <c r="Q34" s="9">
+        <f>+D34-N34</f>
+        <v/>
+      </c>
+      <c r="R34" s="9">
+        <f>+E34-O34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>6</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8380</v>
+      </c>
+      <c r="E35" t="n">
+        <v>50280</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J35" t="n">
+        <v>50280</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>6</v>
+      </c>
+      <c r="N35" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O35" t="n">
+        <v>50280</v>
+      </c>
+      <c r="P35" s="9">
+        <f>+C35-M35</f>
+        <v/>
+      </c>
+      <c r="Q35" s="9">
+        <f>+D35-N35</f>
+        <v/>
+      </c>
+      <c r="R35" s="9">
+        <f>+E35-O35</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="D36" t="n">
+        <v>8380</v>
+      </c>
+      <c r="E36" t="n">
+        <v>97208</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J36" t="n">
+        <v>97208</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N36" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O36" t="n">
+        <v>97208</v>
+      </c>
+      <c r="P36" s="9">
+        <f>+C36-M36</f>
+        <v/>
+      </c>
+      <c r="Q36" s="9">
+        <f>+D36-N36</f>
+        <v/>
+      </c>
+      <c r="R36" s="9">
+        <f>+E36-O36</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D37" t="n">
+        <v>109371.57</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1006218.4</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>109802</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1010178.4</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="N37" t="n">
+        <v>11935</v>
+      </c>
+      <c r="O37" t="n">
+        <v>109802</v>
+      </c>
+      <c r="P37" s="9">
+        <f>+C37-M37</f>
+        <v/>
+      </c>
+      <c r="Q37" s="9">
+        <f>+D37-N37</f>
+        <v/>
+      </c>
+      <c r="R37" s="9">
+        <f>+E37-O37</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>9</v>
+      </c>
+      <c r="D38" t="n">
+        <v>54000</v>
+      </c>
+      <c r="E38" t="n">
+        <v>486000</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>54000</v>
+      </c>
+      <c r="J38" t="n">
+        <v>486000</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>9</v>
+      </c>
+      <c r="N38" t="n">
+        <v>6000</v>
+      </c>
+      <c r="O38" t="n">
+        <v>54000</v>
+      </c>
+      <c r="P38" s="9">
+        <f>+C38-M38</f>
+        <v/>
+      </c>
+      <c r="Q38" s="9">
+        <f>+D38-N38</f>
+        <v/>
+      </c>
+      <c r="R38" s="9">
+        <f>+E38-O38</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CHORIZO PURO CERDO</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D39" t="n">
+        <v>12190</v>
+      </c>
+      <c r="E39" t="n">
+        <v>28037</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>12190</v>
+      </c>
+      <c r="J39" t="n">
+        <v>28037</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>CHORIZO PURO CERDO</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="N39" t="n">
+        <v>5300</v>
+      </c>
+      <c r="O39" t="n">
+        <v>12190</v>
+      </c>
+      <c r="P39" s="9">
+        <f>+C39-M39</f>
+        <v/>
+      </c>
+      <c r="Q39" s="9">
+        <f>+D39-N39</f>
+        <v/>
+      </c>
+      <c r="R39" s="9">
+        <f>+E39-O39</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SUPREMA</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="D40" t="n">
+        <v>7450</v>
+      </c>
+      <c r="E40" t="n">
+        <v>74500</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>COCHINCHINA</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>7450</v>
+      </c>
+      <c r="J40" t="n">
+        <v>74500</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>SUPREMA</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>10</v>
+      </c>
+      <c r="N40" t="n">
+        <v>7450</v>
+      </c>
+      <c r="O40" t="n">
+        <v>74500</v>
+      </c>
+      <c r="P40" s="9">
+        <f>+C40-M40</f>
+        <v/>
+      </c>
+      <c r="Q40" s="9">
+        <f>+D40-N40</f>
+        <v/>
+      </c>
+      <c r="R40" s="9">
+        <f>+E40-O40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>OJO DE BIFE</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="D41" t="n">
+        <v>15535</v>
+      </c>
+      <c r="E41" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Galicia Polo Mince Bar</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>15535</v>
+      </c>
+      <c r="J41" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>OJO DE BIFE</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="N41" t="n">
+        <v>15535</v>
+      </c>
+      <c r="O41" t="n">
+        <v>97870.5</v>
+      </c>
+      <c r="P41" s="9">
+        <f>+C41-M41</f>
+        <v/>
+      </c>
+      <c r="Q41" s="9">
+        <f>+D41-N41</f>
+        <v/>
+      </c>
+      <c r="R41" s="9">
+        <f>+E41-O41</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>6</v>
+      </c>
+      <c r="D42" t="n">
+        <v>6680</v>
+      </c>
+      <c r="E42" t="n">
+        <v>40080</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J42" t="n">
+        <v>50280</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>ROAS BEEF</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>6</v>
+      </c>
+      <c r="N42" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O42" t="n">
+        <v>50280</v>
+      </c>
+      <c r="P42" s="9">
+        <f>+C42-M42</f>
+        <v/>
+      </c>
+      <c r="Q42" s="9">
+        <f>+D42-N42</f>
+        <v/>
+      </c>
+      <c r="R42" s="9">
+        <f>+E42-O42</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="D43" t="n">
+        <v>8380</v>
+      </c>
+      <c r="E43" t="n">
+        <v>97208</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>8380</v>
+      </c>
+      <c r="J43" t="n">
+        <v>97208</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N43" t="n">
+        <v>8380</v>
+      </c>
+      <c r="O43" t="n">
+        <v>97208</v>
+      </c>
+      <c r="P43" s="9">
+        <f>+C43-M43</f>
+        <v/>
+      </c>
+      <c r="Q43" s="9">
+        <f>+D43-N43</f>
+        <v/>
+      </c>
+      <c r="R43" s="9">
+        <f>+E43-O43</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D44" t="n">
+        <v>109375.91</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1006258.4</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>109802</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1010178.4</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>NALGA FETEADA</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="N44" t="n">
+        <v>11935</v>
+      </c>
+      <c r="O44" t="n">
+        <v>109802</v>
+      </c>
+      <c r="P44" s="9">
+        <f>+C44-M44</f>
+        <v/>
+      </c>
+      <c r="Q44" s="9">
+        <f>+D44-N44</f>
+        <v/>
+      </c>
+      <c r="R44" s="9">
+        <f>+E44-O44</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>9</v>
+      </c>
+      <c r="D45" t="n">
+        <v>54000</v>
+      </c>
+      <c r="E45" t="n">
+        <v>486000</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>54000</v>
+      </c>
+      <c r="J45" t="n">
+        <v>486000</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>CARNE PICADA</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>9</v>
+      </c>
+      <c r="N45" t="n">
+        <v>6000</v>
+      </c>
+      <c r="O45" t="n">
+        <v>54000</v>
+      </c>
+      <c r="P45" s="9">
+        <f>+C45-M45</f>
+        <v/>
+      </c>
+      <c r="Q45" s="9">
+        <f>+D45-N45</f>
+        <v/>
+      </c>
+      <c r="R45" s="9">
+        <f>+E45-O45</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CHORIZO PURO CERDO</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D46" t="n">
+        <v>11755.22</v>
+      </c>
+      <c r="E46" t="n">
+        <v>27037</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>LA MALA</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>12190</v>
+      </c>
+      <c r="J46" t="n">
+        <v>28037</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>CHORIZO PURO CERDO</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="N46" t="n">
+        <v>5300</v>
+      </c>
+      <c r="O46" t="n">
+        <v>12190</v>
+      </c>
+      <c r="P46" s="9">
+        <f>+C46-M46</f>
+        <v/>
+      </c>
+      <c r="Q46" s="9">
+        <f>+D46-N46</f>
+        <v/>
+      </c>
+      <c r="R46" s="9">
+        <f>+E46-O46</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SUPREMA</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>10</v>
+      </c>
+      <c r="D47" t="n">
+        <v>7450</v>
+      </c>
+      <c r="E47" t="n">
+        <v>74500</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>COCHINCHINA</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Kunze SRL</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>7450</v>
+      </c>
+      <c r="J47" t="n">
+        <v>74500</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>SUPREMA</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>10</v>
+      </c>
+      <c r="N47" t="n">
+        <v>7450</v>
+      </c>
+      <c r="O47" t="n">
+        <v>74500</v>
+      </c>
+      <c r="P47" s="9">
+        <f>+C47-M47</f>
+        <v/>
+      </c>
+      <c r="Q47" s="9">
+        <f>+D47-N47</f>
+        <v/>
+      </c>
+      <c r="R47" s="9">
+        <f>+E47-O47</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>10</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>KG FILLET DE POLLO</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>30</v>
+      </c>
+      <c r="D48" t="n">
+        <v>7239.82</v>
+      </c>
+      <c r="E48" t="n">
+        <v>217194.6</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>PERSEO &amp; CO S.A.</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>7239.82</v>
+      </c>
+      <c r="J48" t="n">
+        <v>217194.6</v>
+      </c>
+      <c r="K48" t="n">
+        <v>10</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>FILLET DE POLLO</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N48" t="n">
+        <v>7239.82</v>
+      </c>
+      <c r="O48" t="n">
+        <v>217194.6</v>
+      </c>
+      <c r="P48" s="9">
+        <f>+C48-M48</f>
+        <v/>
+      </c>
+      <c r="Q48" s="9">
+        <f>+D48-N48</f>
+        <v/>
+      </c>
+      <c r="R48" s="9">
+        <f>+E48-O48</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>KG POLLO ENTERO A</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>20</v>
+      </c>
+      <c r="D49" t="n">
+        <v>10500</v>
+      </c>
+      <c r="E49" t="n">
+        <v>210000</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>MOJAMA S.A.</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="J49" t="n">
+        <v>210</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>POLLO ENTERO A</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>20000</v>
+      </c>
+      <c r="N49" t="n">
+        <v>3393.67</v>
+      </c>
+      <c r="O49" t="n">
+        <v>67873.39999999999</v>
+      </c>
+      <c r="P49" s="9">
+        <f>+C49-M49</f>
+        <v/>
+      </c>
+      <c r="Q49" s="9">
+        <f>+D49-N49</f>
+        <v/>
+      </c>
+      <c r="R49" s="9">
+        <f>+E49-O49</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>23</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>KG MILANESA/POLLO GRANDE</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>5</v>
+      </c>
+      <c r="D50" t="n">
+        <v>21000</v>
+      </c>
+      <c r="E50" t="n">
+        <v>105000</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>MOJAMA S.A.</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Buenos Ayres Vinos y Bebidas SA</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>21</v>
+      </c>
+      <c r="J50" t="n">
+        <v>105</v>
+      </c>
+      <c r="K50" t="n">
+        <v>23</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>MILANESA/POLLO GRANDE</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>5000</v>
+      </c>
+      <c r="N50" t="n">
+        <v>6281</v>
+      </c>
+      <c r="O50" t="n">
+        <v>31405</v>
+      </c>
+      <c r="P50" s="9">
+        <f>+C50-M50</f>
+        <v/>
+      </c>
+      <c r="Q50" s="9">
+        <f>+D50-N50</f>
+        <v/>
+      </c>
+      <c r="R50" s="9">
+        <f>+E50-O50</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>VINAGRE DE ALCOHOL MENOYO BID. X SLT SIN TACC</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>8</v>
+      </c>
+      <c r="D51" t="n">
+        <v>5125.09</v>
+      </c>
+      <c r="E51" t="n">
+        <v>41000.72</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>PERSEO &amp; CO.S.A.</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Distribuidora el Criollo</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="J51" t="n">
+        <v>41.04</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>VINAGRE DE ALCOHOL MENOYO BID. X 5LT SIN TACC</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>8</v>
+      </c>
+      <c r="N51" t="n">
+        <v>5125.09</v>
+      </c>
+      <c r="O51" t="n">
+        <v>41000.72</v>
+      </c>
+      <c r="P51" s="9">
+        <f>+C51-M51</f>
+        <v/>
+      </c>
+      <c r="Q51" s="9">
+        <f>+D51-N51</f>
+        <v/>
+      </c>
+      <c r="R51" s="9">
+        <f>+E51-O51</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>JAMON COCIDO CAMPO AUSTRAL KG SIN TACC</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>485</v>
+      </c>
+      <c r="D52" t="n">
+        <v>101.79</v>
+      </c>
+      <c r="E52" t="n">
+        <v>49369.94</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>GOURMAND S.A</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Distribuidora el Criollo</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>10.18</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4937.3</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>JAMON COCIDO CAMPO AUSTRAL KG SIN TACC</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="N52" t="n">
+        <v>10179.37</v>
+      </c>
+      <c r="O52" t="n">
+        <v>49369.94</v>
+      </c>
+      <c r="P52" s="9">
+        <f>+C52-M52</f>
+        <v/>
+      </c>
+      <c r="Q52" s="9">
+        <f>+D52-N52</f>
+        <v/>
+      </c>
+      <c r="R52" s="9">
+        <f>+E52-O52</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>171</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Pata Y Muslo De Pollo</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2699.9</v>
+      </c>
+      <c r="E53" t="n">
+        <v>28348.95</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>15 de Noviembre de 1889 Nº 1710 - CP 1130 - Caba</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>26999</v>
+      </c>
+      <c r="J53" t="n">
+        <v>283489.5</v>
+      </c>
+      <c r="K53" t="n">
+        <v>171</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Pata Y Muslo De Pollo</t>
+        </is>
+      </c>
+      <c r="M53" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="N53" t="n">
+        <v>2699.9</v>
+      </c>
+      <c r="O53" t="n">
+        <v>28348.95</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>162</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Filet De Pollo</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="D54" t="n">
+        <v>7649.9</v>
+      </c>
+      <c r="E54" t="n">
+        <v>46664.39</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>15 de Noviembre de 1889 Nº 1710 - CP 1130 - Caba</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>76499</v>
+      </c>
+      <c r="J54" t="n">
+        <v>466643.9</v>
+      </c>
+      <c r="K54" t="n">
+        <v>162</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Filet De Pollo</t>
+        </is>
+      </c>
+      <c r="M54" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="N54" t="n">
+        <v>7649.9</v>
+      </c>
+      <c r="O54" t="n">
+        <v>46664.39</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>171</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Pata Y Muslo De Pollo</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2699.9</v>
+      </c>
+      <c r="E55" t="n">
+        <v>28348.95</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>BAYONNA S.A.</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Diferencia de Precio</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>26999</v>
+      </c>
+      <c r="J55" t="n">
+        <v>283489.5</v>
+      </c>
+      <c r="K55" t="n">
+        <v>171</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Pata Y Muslo De Pollo</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="N55" t="n">
+        <v>2699.9</v>
+      </c>
+      <c r="O55" t="n">
+        <v>28348.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>